<commit_message>
UPD: translated explanation to english.
</commit_message>
<xml_diff>
--- a/Data/Consumption_expenditures_expl.xlsx
+++ b/Data/Consumption_expenditures_expl.xlsx
@@ -37,13 +37,13 @@
     <t xml:space="preserve">he00</t>
   </si>
   <si>
-    <t xml:space="preserve">Visos namų ūkio vartojimo išlaidos (mėnesinės)</t>
+    <t xml:space="preserve">All household consumption expenses (monthly) </t>
   </si>
   <si>
     <t xml:space="preserve">he01</t>
   </si>
   <si>
-    <t xml:space="preserve">Maistas ir nealkoholiniai gėrimai</t>
+    <t xml:space="preserve">Food and non-alcoholic beverages </t>
   </si>
   <si>
     <t xml:space="preserve">he011</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">he012</t>
   </si>
   <si>
-    <t xml:space="preserve">Nealkoholiniai gėrimai</t>
+    <t xml:space="preserve">Non-alcoholic beverages</t>
   </si>
   <si>
     <t xml:space="preserve">he0121</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">he02</t>
   </si>
   <si>
-    <t xml:space="preserve">Alkoholiniai gėrimai, tabakas ir narkotikai</t>
+    <t xml:space="preserve">Alcoholic beverages, tobacco, and drugs</t>
   </si>
   <si>
     <t xml:space="preserve">he021</t>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">he03</t>
   </si>
   <si>
-    <t xml:space="preserve">Apranga ir avalynė</t>
+    <t xml:space="preserve">Clothing and footwear</t>
   </si>
   <si>
     <t xml:space="preserve">he031</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">he04</t>
   </si>
   <si>
-    <t xml:space="preserve">Būstas, vanduo, elektra, dujos ir kitas kuras</t>
+    <t xml:space="preserve">Housing, water, electricity, gas, and other fuels</t>
   </si>
   <si>
     <t xml:space="preserve">he041</t>
@@ -379,7 +379,7 @@
     <t xml:space="preserve">he05</t>
   </si>
   <si>
-    <t xml:space="preserve">Būsto apstatymo, namų ūkio įranga ir kasdienė namų priežiūra</t>
+    <t xml:space="preserve">Furnishings, household equipment, and routine home maintenance</t>
   </si>
   <si>
     <t xml:space="preserve">he051</t>
@@ -490,7 +490,7 @@
     <t xml:space="preserve">he06</t>
   </si>
   <si>
-    <t xml:space="preserve">Sveikata</t>
+    <t xml:space="preserve">Health</t>
   </si>
   <si>
     <t xml:space="preserve">he061</t>
@@ -586,7 +586,7 @@
     <t xml:space="preserve">he07</t>
   </si>
   <si>
-    <t xml:space="preserve">Transportas</t>
+    <t xml:space="preserve">Transport</t>
   </si>
   <si>
     <t xml:space="preserve">he071</t>
@@ -712,7 +712,7 @@
     <t xml:space="preserve">he08</t>
   </si>
   <si>
-    <t xml:space="preserve">Informacija ir ryšiai</t>
+    <t xml:space="preserve">Information and communication</t>
   </si>
   <si>
     <t xml:space="preserve">he081</t>
@@ -814,7 +814,7 @@
     <t xml:space="preserve">he09</t>
   </si>
   <si>
-    <t xml:space="preserve">Poilsis, sportas ir kultūra</t>
+    <t xml:space="preserve">Recreation, sports, and culture</t>
   </si>
   <si>
     <t xml:space="preserve">he091</t>
@@ -1009,7 +1009,7 @@
     <t xml:space="preserve">he10</t>
   </si>
   <si>
-    <t xml:space="preserve">Švietimo paslaugos</t>
+    <t xml:space="preserve">Education services</t>
   </si>
   <si>
     <t xml:space="preserve">he101</t>
@@ -1060,7 +1060,7 @@
     <t xml:space="preserve">he11</t>
   </si>
   <si>
-    <t xml:space="preserve">Restoranai ir apgyvendinimo paslaugos</t>
+    <t xml:space="preserve">Restaurants and accommodation services</t>
   </si>
   <si>
     <t xml:space="preserve">he111</t>
@@ -1093,7 +1093,7 @@
     <t xml:space="preserve">he12</t>
   </si>
   <si>
-    <t xml:space="preserve">Draudimas ir finansinės paslaugos</t>
+    <t xml:space="preserve">Insurance and financial services</t>
   </si>
   <si>
     <t xml:space="preserve">he121</t>
@@ -1147,7 +1147,7 @@
     <t xml:space="preserve">he13</t>
   </si>
   <si>
-    <t xml:space="preserve">Asmens priežiūra, socialinė apsauga ir įvairios prekės ir paslaugos</t>
+    <t xml:space="preserve">Personal care, social protection, and miscellaneous goods and services</t>
   </si>
   <si>
     <t xml:space="preserve">he131</t>
@@ -1294,12 +1294,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1429,7 +1433,7 @@
   <dimension ref="A1:B207"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1450,19 +1454,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1546,7 +1550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1722,7 +1726,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>68</v>
       </c>
@@ -1794,7 +1798,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
@@ -2082,7 +2086,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
         <v>155</v>
       </c>
@@ -2210,7 +2214,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="s">
         <v>187</v>
       </c>
@@ -2378,7 +2382,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
         <v>229</v>
       </c>
@@ -2778,7 +2782,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
         <v>328</v>
       </c>
@@ -2866,7 +2870,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="46" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
         <v>345</v>
       </c>

</xml_diff>